<commit_message>
for discussion with pidsg 2512
</commit_message>
<xml_diff>
--- a/pidsg26Evaluation12.xlsx
+++ b/pidsg26Evaluation12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debdeeppaul/Documents/Procurement/PIDSG26/pricesaa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E42C02-AAFC-364B-976D-5C6CB67E96AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF824C2-9AD7-424E-B2A5-12A6F2BA5870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="780" windowWidth="28800" windowHeight="15680" tabRatio="500" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" tabRatio="500" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="from_alvin" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="126">
   <si>
     <t>FY24</t>
   </si>
@@ -424,6 +424,9 @@
   <si>
     <t>Manual KUSD</t>
   </si>
+  <si>
+    <t>%age impr</t>
+  </si>
 </sst>
 </file>
 
@@ -482,7 +485,7 @@
       <name val="Aptos Narrow"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +508,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -549,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -597,6 +612,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -18589,8 +18609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC1B279-E546-9F42-8686-CEC74C725A9F}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19570,18 +19590,25 @@
       <c r="C29" s="17">
         <v>50</v>
       </c>
-      <c r="J29" t="s">
+      <c r="I29" s="8"/>
+      <c r="J29" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="30" t="s">
         <v>34</v>
+      </c>
+      <c r="L29" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="M29" s="30" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="C30" s="17">
         <v>52</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="31" t="s">
         <v>50</v>
       </c>
       <c r="J30">
@@ -19605,7 +19632,7 @@
       <c r="C31" s="17">
         <v>53</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="31" t="s">
         <v>57</v>
       </c>
       <c r="J31">
@@ -19633,7 +19660,7 @@
       <c r="C32" s="17">
         <v>54</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="31" t="s">
         <v>75</v>
       </c>
       <c r="J32">
@@ -19651,7 +19678,7 @@
       <c r="C33" s="17">
         <v>55</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="31" t="s">
         <v>18</v>
       </c>
       <c r="J33">
@@ -19666,7 +19693,7 @@
         <f t="shared" si="10"/>
         <v>5.8778513660688692</v>
       </c>
-      <c r="M33" s="9">
+      <c r="M33" s="29">
         <f>SUM(M30:M31)</f>
         <v>72.864625543423529</v>
       </c>

</xml_diff>